<commit_message>
auto building semi-working stable
</commit_message>
<xml_diff>
--- a/shipData/ships.xlsx
+++ b/shipData/ships.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jilek\Documents\Azur-Lane-Fllet-Builder-Dev\shipData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1117AEB-D11C-4D09-9ABE-DD49412E9F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52184C6-C885-426B-BF18-03A898C604E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="432" windowWidth="25860" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2727,8 +2727,8 @@
   <dimension ref="A1:X535"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V191" sqref="V191"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W114" sqref="W114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9647,7 +9647,7 @@
         <v>18</v>
       </c>
       <c r="W114" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="115" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>